<commit_message>
cleaning up gcc activity data
</commit_message>
<xml_diff>
--- a/data/ClimateChangeSigns.xlsx
+++ b/data/ClimateChangeSigns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chc02006/Documents/Teaching/EA30/Fall2021/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54760A8-2CF7-014F-A3F7-79438F07A55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6DD5BC-34B4-DA47-95E3-F564E78287DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="500" windowWidth="27760" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37780" yWindow="-10000" windowWidth="27760" windowHeight="17500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Keeling" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>mean</t>
   </si>
   <si>
     <t>extent</t>
@@ -44,9 +41,6 @@
     <t>TempSmoothed5Yrs</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>NOAASea</t>
   </si>
   <si>
@@ -55,12 +49,15 @@
   <si>
     <t>For tab 4 (OceanHeat), the source was https://www.epa.gov/climate-indicators/climate-change-indicators-ocean-heat</t>
   </si>
+  <si>
+    <t>meanCO2ppm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -79,6 +76,12 @@
       <u/>
       <sz val="10"/>
       <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -104,12 +107,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -331,7 +335,9 @@
   </sheetPr>
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -340,7 +346,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -860,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1211,19 +1217,21 @@
   </sheetPr>
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1986,13 +1994,10 @@
       <c r="A60" s="1">
         <v>1938</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D60" s="2">
+      <c r="B60" s="2">
+        <v>0</v>
+      </c>
+      <c r="C60" s="2">
         <v>-0.01</v>
       </c>
       <c r="E60" s="2"/>
@@ -2004,1308 +2009,1063 @@
       <c r="B61" s="2">
         <v>-0.02</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D61" s="2">
+      <c r="C61" s="2">
         <v>0.03</v>
       </c>
       <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A62" s="1">
+      <c r="A62" s="5">
         <v>1940</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="2">
+      <c r="B62" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="C62" s="5">
         <v>0.06</v>
       </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A63" s="1">
+      <c r="A63" s="5">
         <v>1941</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" s="2">
+      <c r="B63" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="C63" s="5">
         <v>0.09</v>
       </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A64" s="1">
+      <c r="A64" s="5">
         <v>1942</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="2">
+      <c r="B64" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C64" s="5">
         <v>0.11</v>
       </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A65" s="1">
+      <c r="A65" s="5">
         <v>1943</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" s="2">
+      <c r="B65" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="C65" s="5">
         <v>0.1</v>
       </c>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
     </row>
     <row r="66" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A66" s="1">
+      <c r="A66" s="5">
         <v>1944</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" s="2">
+      <c r="B66" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="C66" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A67" s="1">
+      <c r="A67" s="5">
         <v>1945</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" s="2">
+      <c r="B67" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="C67" s="5">
         <v>0.04</v>
       </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A68" s="1">
+      <c r="A68" s="5">
         <v>1946</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D68" s="2">
+      <c r="C68" s="5">
         <v>0</v>
       </c>
+      <c r="D68" s="2"/>
       <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A69" s="1">
+      <c r="A69" s="5">
         <v>1947</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="5">
         <v>-0.03</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="5">
         <v>-0.04</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A70" s="1">
+      <c r="A70" s="5">
         <v>1948</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="5">
         <v>-0.11</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A71" s="1">
+      <c r="A71" s="5">
         <v>1949</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="5">
         <v>-0.11</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="5">
         <v>-0.08</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A72" s="1">
+      <c r="A72" s="5">
         <v>1950</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="5">
         <v>-0.17</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="5">
         <v>-0.08</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A73" s="1">
+      <c r="A73" s="5">
         <v>1951</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A74" s="1">
+      <c r="A74" s="5">
         <v>1952</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" s="2">
+      <c r="B74" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C74" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
+      <c r="D74" s="2"/>
       <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A75" s="1">
+      <c r="A75" s="5">
         <v>1953</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="2">
+      <c r="B75" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="C75" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
+      <c r="D75" s="2"/>
       <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A76" s="1">
+      <c r="A76" s="5">
         <v>1954</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="5">
         <v>-0.13</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A77" s="1">
+      <c r="A77" s="5">
         <v>1955</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="5">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="5">
         <v>-0.06</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A78" s="1">
+      <c r="A78" s="5">
         <v>1956</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="5">
         <v>-0.19</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="5">
         <v>-0.05</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A79" s="1">
+      <c r="A79" s="5">
         <v>1957</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D79" s="2">
+      <c r="B79" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C79" s="5">
         <v>-0.04</v>
       </c>
+      <c r="D79" s="2"/>
       <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A80" s="1">
+      <c r="A80" s="5">
         <v>1958</v>
       </c>
-      <c r="B80" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D80" s="2">
+      <c r="B80" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="C80" s="5">
         <v>-0.01</v>
       </c>
+      <c r="D80" s="2"/>
       <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A81" s="1">
+      <c r="A81" s="5">
         <v>1959</v>
       </c>
-      <c r="B81" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E81" s="2">
+      <c r="B81" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="C81" s="5">
         <v>0.01</v>
       </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A82" s="1">
+      <c r="A82" s="5">
         <v>1960</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="5">
         <v>-0.03</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="2">
+      <c r="C82" s="5">
         <v>0.03</v>
       </c>
+      <c r="D82" s="2"/>
       <c r="E82" s="2"/>
     </row>
     <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A83" s="1">
+      <c r="A83" s="5">
         <v>1961</v>
       </c>
-      <c r="B83" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E83" s="2">
+      <c r="B83" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="C83" s="5">
         <v>0.01</v>
       </c>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
     </row>
     <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A84" s="1">
+      <c r="A84" s="5">
         <v>1962</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" s="2">
+      <c r="B84" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="C84" s="5">
         <v>-0.01</v>
       </c>
+      <c r="D84" s="2"/>
       <c r="E84" s="2"/>
     </row>
     <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A85" s="1">
+      <c r="A85" s="5">
         <v>1963</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D85" s="2">
+      <c r="B85" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C85" s="5">
         <v>-0.03</v>
       </c>
+      <c r="D85" s="2"/>
       <c r="E85" s="2"/>
     </row>
     <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A86" s="1">
+      <c r="A86" s="5">
         <v>1964</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="5">
         <v>-0.2</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="5">
         <v>-0.04</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A87" s="1">
+      <c r="A87" s="5">
         <v>1965</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="5">
         <v>-0.11</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="5">
         <v>-0.05</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A88" s="1">
+      <c r="A88" s="5">
         <v>1966</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="5">
         <v>-0.06</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="5">
         <v>-0.06</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A89" s="1">
+      <c r="A89" s="5">
         <v>1967</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="5">
         <v>-0.02</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="5">
         <v>-0.05</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A90" s="1">
+      <c r="A90" s="5">
         <v>1968</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="5">
         <v>-0.08</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90" s="5">
         <v>-0.03</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A91" s="1">
+      <c r="A91" s="5">
         <v>1969</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D91" s="2">
+      <c r="B91" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C91" s="5">
         <v>-0.02</v>
       </c>
+      <c r="D91" s="2"/>
       <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A92" s="1">
+      <c r="A92" s="5">
         <v>1970</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D92" s="2">
+      <c r="B92" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="C92" s="5">
         <v>0</v>
       </c>
+      <c r="D92" s="2"/>
       <c r="E92" s="2"/>
     </row>
     <row r="93" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A93" s="1">
+      <c r="A93" s="5">
         <v>1971</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="5">
         <v>-0.08</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D93" s="2">
+      <c r="C93" s="5">
         <v>0</v>
       </c>
+      <c r="D93" s="2"/>
       <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A94" s="1">
+      <c r="A94" s="5">
         <v>1972</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E94" s="2">
+      <c r="B94" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C94" s="5">
         <v>0</v>
       </c>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
     </row>
     <row r="95" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A95" s="1">
+      <c r="A95" s="5">
         <v>1973</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" s="2">
+      <c r="B95" s="5">
+        <v>0.16</v>
+      </c>
+      <c r="C95" s="5">
         <v>0</v>
       </c>
+      <c r="D95" s="2"/>
       <c r="E95" s="2"/>
     </row>
     <row r="96" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A96" s="1">
+      <c r="A96" s="5">
         <v>1974</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="5">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" s="2">
+      <c r="C96" s="5">
         <v>0.01</v>
       </c>
+      <c r="D96" s="2"/>
       <c r="E96" s="2"/>
     </row>
     <row r="97" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A97" s="1">
+      <c r="A97" s="5">
         <v>1975</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="5">
         <v>-0.01</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D97" s="2">
+      <c r="C97" s="5">
         <v>0.02</v>
       </c>
+      <c r="D97" s="2"/>
       <c r="E97" s="2"/>
     </row>
     <row r="98" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A98" s="1">
+      <c r="A98" s="5">
         <v>1976</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="5">
         <v>-0.1</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" s="2">
+      <c r="C98" s="5">
         <v>0.04</v>
       </c>
+      <c r="D98" s="2"/>
       <c r="E98" s="2"/>
     </row>
     <row r="99" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A99" s="1">
+      <c r="A99" s="5">
         <v>1977</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E99" s="2">
+      <c r="B99" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="C99" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
     </row>
     <row r="100" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A100" s="1">
+      <c r="A100" s="5">
         <v>1978</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" s="2">
+      <c r="B100" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C100" s="5">
         <v>0.12</v>
       </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
     </row>
     <row r="101" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A101" s="1">
+      <c r="A101" s="5">
         <v>1979</v>
       </c>
-      <c r="B101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="2">
+      <c r="B101" s="5">
         <v>0.16</v>
       </c>
+      <c r="C101" s="5">
+        <v>0.16</v>
+      </c>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
     </row>
     <row r="102" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A102" s="1">
+      <c r="A102" s="5">
         <v>1980</v>
       </c>
-      <c r="B102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" s="2">
+      <c r="B102" s="5">
+        <v>0.26</v>
+      </c>
+      <c r="C102" s="5">
         <v>0.2</v>
       </c>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
     </row>
     <row r="103" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A103" s="1">
+      <c r="A103" s="5">
         <v>1981</v>
       </c>
-      <c r="B103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E103" s="2">
+      <c r="B103" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="C103" s="5">
         <v>0.21</v>
       </c>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
     </row>
     <row r="104" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A104" s="1">
+      <c r="A104" s="5">
         <v>1982</v>
       </c>
-      <c r="B104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E104" s="2">
+      <c r="B104" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C104" s="5">
         <v>0.22</v>
       </c>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
     </row>
     <row r="105" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A105" s="1">
+      <c r="A105" s="5">
         <v>1983</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E105" s="2">
+      <c r="B105" s="5">
+        <v>0.31</v>
+      </c>
+      <c r="C105" s="5">
         <v>0.21</v>
       </c>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A106" s="1">
+      <c r="A106" s="5">
         <v>1984</v>
       </c>
-      <c r="B106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E106" s="2">
+      <c r="B106" s="5">
+        <v>0.16</v>
+      </c>
+      <c r="C106" s="5">
         <v>0.21</v>
       </c>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A107" s="1">
+      <c r="A107" s="5">
         <v>1985</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E107" s="2">
+      <c r="B107" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="C107" s="5">
         <v>0.22</v>
       </c>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A108" s="1">
+      <c r="A108" s="5">
         <v>1986</v>
       </c>
-      <c r="B108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E108" s="2">
+      <c r="B108" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="C108" s="5">
         <v>0.24</v>
       </c>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
     </row>
     <row r="109" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A109" s="1">
+      <c r="A109" s="5">
         <v>1987</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E109" s="2">
+      <c r="B109" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="C109" s="5">
         <v>0.27</v>
       </c>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A110" s="1">
+      <c r="A110" s="5">
         <v>1988</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E110" s="2">
+      <c r="B110" s="5">
+        <v>0.39</v>
+      </c>
+      <c r="C110" s="5">
         <v>0.31</v>
       </c>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
     </row>
     <row r="111" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A111" s="1">
+      <c r="A111" s="5">
         <v>1989</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E111" s="2">
+      <c r="B111" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="C111" s="5">
         <v>0.33</v>
       </c>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
     </row>
     <row r="112" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A112" s="1">
+      <c r="A112" s="5">
         <v>1990</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E112" s="2">
+      <c r="B112" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="C112" s="5">
         <v>0.33</v>
       </c>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A113" s="1">
+      <c r="A113" s="5">
         <v>1991</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E113" s="2">
+      <c r="B113" s="5">
+        <v>0.41</v>
+      </c>
+      <c r="C113" s="5">
         <v>0.33</v>
       </c>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A114" s="1">
+      <c r="A114" s="5">
         <v>1992</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E114" s="2">
+      <c r="B114" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="C114" s="5">
         <v>0.33</v>
       </c>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A115" s="1">
+      <c r="A115" s="5">
         <v>1993</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E115" s="2">
+      <c r="B115" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="C115" s="5">
         <v>0.33</v>
       </c>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
     </row>
     <row r="116" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A116" s="1">
+      <c r="A116" s="5">
         <v>1994</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E116" s="2">
+      <c r="B116" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="C116" s="5">
         <v>0.34</v>
       </c>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
     </row>
     <row r="117" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A117" s="1">
+      <c r="A117" s="5">
         <v>1995</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E117" s="2">
+      <c r="B117" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="C117" s="5">
         <v>0.37</v>
       </c>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
     </row>
     <row r="118" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A118" s="1">
+      <c r="A118" s="5">
         <v>1996</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E118" s="2">
+      <c r="B118" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="C118" s="5">
         <v>0.4</v>
       </c>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
     </row>
     <row r="119" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A119" s="1">
+      <c r="A119" s="5">
         <v>1997</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E119" s="2">
+      <c r="B119" s="5">
+        <v>0.46</v>
+      </c>
+      <c r="C119" s="5">
         <v>0.42</v>
       </c>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
     </row>
     <row r="120" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A120" s="1">
+      <c r="A120" s="5">
         <v>1998</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E120" s="2">
+      <c r="B120" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="C120" s="5">
         <v>0.45</v>
       </c>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
     </row>
     <row r="121" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A121" s="1">
+      <c r="A121" s="5">
         <v>1999</v>
       </c>
-      <c r="B121" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E121" s="2">
+      <c r="B121" s="5">
+        <v>0.38</v>
+      </c>
+      <c r="C121" s="5">
         <v>0.47</v>
       </c>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
     </row>
     <row r="122" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A122" s="1">
+      <c r="A122" s="5">
         <v>2000</v>
       </c>
-      <c r="B122" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E122" s="2">
+      <c r="B122" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C122" s="5">
         <v>0.5</v>
       </c>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
     </row>
     <row r="123" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A123" s="1">
+      <c r="A123" s="5">
         <v>2001</v>
       </c>
-      <c r="B123" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C123" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D123" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E123" s="2">
+      <c r="B123" s="5">
+        <v>0.54</v>
+      </c>
+      <c r="C123" s="5">
         <v>0.52</v>
       </c>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
     </row>
     <row r="124" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A124" s="1">
+      <c r="A124" s="5">
         <v>2002</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D124" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E124" s="2">
+      <c r="B124" s="5">
+        <v>0.63</v>
+      </c>
+      <c r="C124" s="5">
         <v>0.55000000000000004</v>
       </c>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
     </row>
     <row r="125" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A125" s="1">
+      <c r="A125" s="5">
         <v>2003</v>
       </c>
-      <c r="B125" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D125" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E125" s="2">
+      <c r="B125" s="5">
+        <v>0.62</v>
+      </c>
+      <c r="C125" s="5">
         <v>0.59</v>
       </c>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
     </row>
     <row r="126" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A126" s="1">
+      <c r="A126" s="5">
         <v>2004</v>
       </c>
-      <c r="B126" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E126" s="2">
+      <c r="B126" s="5">
+        <v>0.54</v>
+      </c>
+      <c r="C126" s="5">
         <v>0.61</v>
       </c>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
     </row>
     <row r="127" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A127" s="1">
+      <c r="A127" s="5">
         <v>2005</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D127" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E127" s="2">
+      <c r="B127" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="C127" s="5">
         <v>0.62</v>
       </c>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
     </row>
     <row r="128" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A128" s="1">
+      <c r="A128" s="5">
         <v>2006</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D128" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E128" s="2">
+      <c r="B128" s="5">
+        <v>0.64</v>
+      </c>
+      <c r="C128" s="5">
         <v>0.63</v>
       </c>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
     </row>
     <row r="129" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A129" s="1">
+      <c r="A129" s="5">
         <v>2007</v>
       </c>
-      <c r="B129" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C129" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D129" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E129" s="2">
+      <c r="B129" s="5">
+        <v>0.67</v>
+      </c>
+      <c r="C129" s="5">
         <v>0.64</v>
       </c>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
     </row>
     <row r="130" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A130" s="1">
+      <c r="A130" s="5">
         <v>2008</v>
       </c>
-      <c r="B130" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E130" s="2">
+      <c r="B130" s="5">
+        <v>0.54</v>
+      </c>
+      <c r="C130" s="5">
         <v>0.64</v>
       </c>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
     </row>
     <row r="131" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A131" s="1">
+      <c r="A131" s="5">
         <v>2009</v>
       </c>
-      <c r="B131" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E131" s="2">
+      <c r="B131" s="5">
+        <v>0.66</v>
+      </c>
+      <c r="C131" s="5">
         <v>0.64</v>
       </c>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
     </row>
     <row r="132" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A132" s="1">
+      <c r="A132" s="5">
         <v>2010</v>
       </c>
-      <c r="B132" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C132" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E132" s="2">
+      <c r="B132" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="C132" s="5">
         <v>0.65</v>
       </c>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
     </row>
     <row r="133" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A133" s="1">
+      <c r="A133" s="5">
         <v>2011</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E133" s="2">
+      <c r="B133" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="C133" s="5">
         <v>0.67</v>
       </c>
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
     </row>
     <row r="134" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A134" s="1">
+      <c r="A134" s="5">
         <v>2012</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E134" s="2">
+      <c r="B134" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="C134" s="5">
         <v>0.7</v>
       </c>
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
     </row>
     <row r="135" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A135" s="1">
+      <c r="A135" s="5">
         <v>2013</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E135" s="2">
+      <c r="B135" s="5">
+        <v>0.68</v>
+      </c>
+      <c r="C135" s="5">
         <v>0.74</v>
       </c>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
     </row>
     <row r="136" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A136" s="1">
+      <c r="A136" s="5">
         <v>2014</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E136" s="2">
+      <c r="B136" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="C136" s="5">
         <v>0.79</v>
       </c>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
     </row>
     <row r="137" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A137" s="1">
+      <c r="A137" s="5">
         <v>2015</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D137" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E137" s="2">
+      <c r="B137" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="C137" s="5">
         <v>0.83</v>
       </c>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
     </row>
     <row r="138" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A138" s="1">
+      <c r="A138" s="5">
         <v>2016</v>
       </c>
-      <c r="B138" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E138" s="2">
+      <c r="B138" s="5">
+        <v>1.02</v>
+      </c>
+      <c r="C138" s="5">
         <v>0.88</v>
       </c>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
     </row>
     <row r="139" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A139" s="1">
+      <c r="A139" s="5">
         <v>2017</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D139" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E139" s="2">
+      <c r="B139" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="C139" s="5">
         <v>0.91</v>
       </c>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
     </row>
     <row r="140" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A140" s="1">
+      <c r="A140" s="5">
         <v>2018</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D140" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E140" s="2">
+      <c r="B140" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="C140" s="5">
         <v>0.95</v>
       </c>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
     </row>
     <row r="141" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A141" s="1">
+      <c r="A141" s="5">
         <v>2019</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D141" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E141" s="2">
+      <c r="B141" s="5">
         <v>0.98</v>
       </c>
+      <c r="C141" s="5">
+        <v>0.98</v>
+      </c>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
     </row>
     <row r="142" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A142" s="1">
+      <c r="A142" s="5">
         <v>2020</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D142" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E142" s="2">
+      <c r="B142" s="5">
+        <v>1.02</v>
+      </c>
+      <c r="C142" s="5">
         <v>1.01</v>
       </c>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3319,16 +3079,18 @@
   </sheetPr>
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3868,7 +3630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBD96D36-79E6-7049-AC49-10F39D422ED6}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -3876,12 +3638,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>